<commit_message>
Minutes and backlog updates
</commit_message>
<xml_diff>
--- a/SprintBacklog/Sprint5.xlsx
+++ b/SprintBacklog/Sprint5.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="35">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -246,7 +246,14 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="110">
+  <dxfs count="66">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -278,13 +285,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -313,6 +313,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -334,13 +341,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -369,6 +369,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -390,13 +397,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -614,13 +614,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -692,307 +685,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1028,8 +720,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="109"/>
-      <tableStyleElement type="headerRow" dxfId="108"/>
+      <tableStyleElement type="wholeTable" dxfId="65"/>
+      <tableStyleElement type="headerRow" dxfId="64"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1338,7 +1030,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:R19"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2074,22 +1766,54 @@
       <c r="B20" s="3">
         <v>60</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
+      <c r="C20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="3">
+        <v>60</v>
+      </c>
+      <c r="E20" s="3">
+        <v>60</v>
+      </c>
+      <c r="F20" s="3">
+        <v>60</v>
+      </c>
+      <c r="G20" s="3">
+        <v>60</v>
+      </c>
+      <c r="H20" s="3">
+        <v>60</v>
+      </c>
+      <c r="I20" s="3">
+        <v>60</v>
+      </c>
+      <c r="J20" s="3">
+        <v>60</v>
+      </c>
+      <c r="K20" s="3">
+        <v>60</v>
+      </c>
+      <c r="L20" s="3">
+        <v>60</v>
+      </c>
+      <c r="M20" s="3">
+        <v>30</v>
+      </c>
+      <c r="N20" s="3">
+        <v>0</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
@@ -2098,46 +1822,110 @@
       <c r="B21" s="3">
         <v>100</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
+      <c r="C21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="3">
+        <v>100</v>
+      </c>
+      <c r="E21" s="3">
+        <v>100</v>
+      </c>
+      <c r="F21" s="3">
+        <v>100</v>
+      </c>
+      <c r="G21" s="3">
+        <v>100</v>
+      </c>
+      <c r="H21" s="3">
+        <v>100</v>
+      </c>
+      <c r="I21" s="3">
+        <v>100</v>
+      </c>
+      <c r="J21" s="3">
+        <v>100</v>
+      </c>
+      <c r="K21" s="3">
+        <v>100</v>
+      </c>
+      <c r="L21" s="3">
+        <v>100</v>
+      </c>
+      <c r="M21" s="3">
+        <v>100</v>
+      </c>
+      <c r="N21" s="3">
+        <v>100</v>
+      </c>
+      <c r="O21" s="3">
+        <v>50</v>
+      </c>
+      <c r="P21" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="3">
-        <v>40</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
+        <v>120</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="3">
+        <v>120</v>
+      </c>
+      <c r="E22" s="3">
+        <v>120</v>
+      </c>
+      <c r="F22" s="3">
+        <v>120</v>
+      </c>
+      <c r="G22" s="3">
+        <v>120</v>
+      </c>
+      <c r="H22" s="3">
+        <v>120</v>
+      </c>
+      <c r="I22" s="3">
+        <v>120</v>
+      </c>
+      <c r="J22" s="3">
+        <v>120</v>
+      </c>
+      <c r="K22" s="3">
+        <v>120</v>
+      </c>
+      <c r="L22" s="3">
+        <v>120</v>
+      </c>
+      <c r="M22" s="3">
+        <v>120</v>
+      </c>
+      <c r="N22" s="3">
+        <v>120</v>
+      </c>
+      <c r="O22" s="3">
+        <v>120</v>
+      </c>
+      <c r="P22" s="3">
+        <v>120</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>120</v>
+      </c>
+      <c r="R22" s="3">
+        <v>120</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
@@ -2298,67 +2086,67 @@
       </c>
       <c r="B29">
         <f>SUM(B4:B25)</f>
-        <v>292</v>
+        <v>372</v>
       </c>
       <c r="D29">
         <f>SUM(D4:D28)</f>
-        <v>92</v>
+        <v>372</v>
       </c>
       <c r="E29">
-        <f>SUM(E4:E25)</f>
-        <v>60</v>
+        <f t="shared" ref="E29:J29" si="0">SUM(E4:E25)</f>
+        <v>340</v>
       </c>
       <c r="F29">
-        <f>SUM(F4:F25)</f>
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>340</v>
       </c>
       <c r="G29">
-        <f>SUM(G4:G25)</f>
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>340</v>
       </c>
       <c r="H29">
-        <f>SUM(H4:H25)</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>320</v>
       </c>
       <c r="I29">
-        <f>SUM(I4:I25)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>280</v>
       </c>
       <c r="J29">
-        <f>SUM(J4:J25)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>280</v>
       </c>
       <c r="K29">
-        <f>SUM(K4:K28)</f>
-        <v>0</v>
+        <f t="shared" ref="K29:Q29" si="1">SUM(K4:K28)</f>
+        <v>280</v>
       </c>
       <c r="L29">
-        <f>SUM(L4:L28)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>280</v>
       </c>
       <c r="M29">
-        <f>SUM(M4:M28)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>250</v>
       </c>
       <c r="N29">
-        <f>SUM(N4:N28)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>220</v>
       </c>
       <c r="O29">
-        <f>SUM(O4:O28)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>170</v>
       </c>
       <c r="P29">
-        <f>SUM(P4:P28)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>130</v>
       </c>
       <c r="Q29">
-        <f>SUM(Q4:Q28)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="R29">
         <f>SUM(R1:R25)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -2368,162 +2156,210 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="83" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="113" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" dxfId="82" priority="98" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="62" priority="110" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="99" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="61" priority="111" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="100" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="60" priority="112" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="79" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="109" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="78" priority="94" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="58" priority="106" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="95" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="57" priority="107" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="96" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="56" priority="108" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="75" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="105" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" dxfId="74" priority="102" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="54" priority="114" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="103" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="53" priority="115" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="104" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="52" priority="116" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="containsText" dxfId="55" priority="30" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="51" priority="42" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="31" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="50" priority="43" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="32" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="49" priority="44" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="52" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="41" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="47" priority="22" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="47" priority="34" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="23" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="46" priority="35" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="24" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="45" priority="36" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="44" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="33" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="43" priority="18" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="43" priority="30" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="19" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="42" priority="31" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="41" priority="32" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="40" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="29" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="containsText" dxfId="39" priority="14" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="39" priority="26" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="15" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="38" priority="27" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="16" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="37" priority="28" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="36" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="25" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="35" priority="10" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="35" priority="22" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="34" priority="23" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="33" priority="24" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="32" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="21" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="27" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="29" priority="16" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="13" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="27" priority="18" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="17" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2531,7 +2367,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3">
       <formula1>To_Do</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:C28 C7 C10:C12 C15:C17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:C28 C7 C10:C12 C15:C17 C20:C22">
       <formula1>Todos</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>